<commit_message>
add missing data to heval3
</commit_message>
<xml_diff>
--- a/data/raw/Human_Evaluation_Results_3rd.xlsx
+++ b/data/raw/Human_Evaluation_Results_3rd.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\einsortieren\_DATA\Uni\WWU\master\19_wise2425\Aligning AI\project\_orga\allocate\finished_heval3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\einsortieren\_DATA\Uni\WWU\master\19_wise2425\Aligning AI\project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6815580-2FF0-403F-AA49-5DEEEF3EDE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74128F66-5C33-4CB6-A2CF-F45B8E0962F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4128" yWindow="-17388" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,18 +458,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,14 +685,14 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.81640625" customWidth="1"/>
     <col min="3" max="3" width="43.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="7" customWidth="1"/>
     <col min="5" max="26" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -709,7 +706,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -769,7 +766,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -779,7 +776,7 @@
       <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="3">
@@ -831,7 +828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -841,7 +838,7 @@
       <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="3">
@@ -893,7 +890,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -903,7 +900,7 @@
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="3">
@@ -955,7 +952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -965,7 +962,7 @@
       <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="3">
@@ -1017,7 +1014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1024,7 @@
       <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="3">
@@ -1079,7 +1076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1089,7 +1086,7 @@
       <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="3">
@@ -1151,7 +1148,7 @@
       <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E8">
@@ -1213,7 +1210,7 @@
       <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E9">
@@ -1278,7 +1275,7 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E10">
@@ -1343,7 +1340,7 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E11">
@@ -1408,7 +1405,7 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E12">
@@ -1473,7 +1470,7 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E13">
@@ -1538,7 +1535,7 @@
       <c r="C14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E14">
@@ -1603,7 +1600,7 @@
       <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E15">
@@ -1665,7 +1662,7 @@
       <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E16">
@@ -1730,7 +1727,7 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E17">
@@ -1795,7 +1792,7 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E18">
@@ -1860,7 +1857,7 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E19">
@@ -1925,7 +1922,7 @@
       <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E20">
@@ -1990,7 +1987,7 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>72</v>
       </c>
       <c r="E21">
@@ -2055,7 +2052,7 @@
       <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E22">
@@ -2120,11 +2117,11 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2185,7 +2182,7 @@
       <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>79</v>
       </c>
       <c r="E24">
@@ -2250,7 +2247,7 @@
       <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E25">
@@ -2312,11 +2309,11 @@
       <c r="C26" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>84</v>
       </c>
       <c r="E26">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2377,7 +2374,7 @@
       <c r="C27" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E27">
@@ -2442,7 +2439,7 @@
       <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>90</v>
       </c>
       <c r="E28">
@@ -2507,7 +2504,7 @@
       <c r="C29" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>93</v>
       </c>
       <c r="E29">
@@ -2569,11 +2566,11 @@
       <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2631,7 +2628,7 @@
       <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E31">
@@ -2690,7 +2687,7 @@
       <c r="C32" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F32">
@@ -2749,7 +2746,7 @@
       <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E33">
@@ -2811,7 +2808,7 @@
       <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E34">
@@ -2873,7 +2870,7 @@
       <c r="C35" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E35">
@@ -2938,7 +2935,7 @@
       <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>108</v>
       </c>
       <c r="E36">
@@ -3000,7 +2997,7 @@
       <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E37">
@@ -3062,7 +3059,7 @@
       <c r="C38" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>112</v>
       </c>
       <c r="E38">
@@ -3117,319 +3114,319 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="7">
         <v>86</v>
       </c>
-      <c r="E39" s="6">
-        <v>1</v>
-      </c>
-      <c r="F39" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G39" s="6">
-        <v>0</v>
-      </c>
-      <c r="H39" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I39" s="6">
-        <v>0</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="6">
-        <v>0</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M39" s="6">
-        <v>-1</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O39" s="6">
-        <v>-1</v>
-      </c>
-      <c r="P39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R39" s="6">
-        <v>0</v>
-      </c>
-      <c r="S39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U39" s="6" t="s">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>-1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>-1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M39">
+        <v>-1</v>
+      </c>
+      <c r="N39" t="s">
+        <v>25</v>
+      </c>
+      <c r="O39">
+        <v>-1</v>
+      </c>
+      <c r="P39" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>25</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39" t="s">
+        <v>25</v>
+      </c>
+      <c r="U39" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="7">
         <v>153</v>
       </c>
-      <c r="E40" s="6">
-        <v>1</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="6">
-        <v>-1</v>
-      </c>
-      <c r="H40" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I40" s="6">
-        <v>0</v>
-      </c>
-      <c r="J40" s="6">
-        <v>-1</v>
-      </c>
-      <c r="K40" s="6">
-        <v>0</v>
-      </c>
-      <c r="L40" s="6">
-        <v>0</v>
-      </c>
-      <c r="M40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N40" s="6">
-        <v>0</v>
-      </c>
-      <c r="O40" s="6">
-        <v>-1</v>
-      </c>
-      <c r="P40" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>0</v>
-      </c>
-      <c r="R40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U40" s="6" t="s">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <v>-1</v>
+      </c>
+      <c r="H40">
+        <v>-1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>-1</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>25</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>-1</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40" t="s">
+        <v>25</v>
+      </c>
+      <c r="S40" t="s">
+        <v>25</v>
+      </c>
+      <c r="U40" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="7">
         <v>42</v>
       </c>
-      <c r="E41" s="6">
-        <v>1</v>
-      </c>
-      <c r="F41" s="6">
-        <v>0</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J41" s="6">
-        <v>0</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="6">
-        <v>0</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O41" s="6">
-        <v>-1</v>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U41" s="6" t="s">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41">
+        <v>-1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41" t="s">
+        <v>25</v>
+      </c>
+      <c r="O41">
+        <v>-1</v>
+      </c>
+      <c r="P41" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>25</v>
+      </c>
+      <c r="R41" t="s">
+        <v>25</v>
+      </c>
+      <c r="S41" t="s">
+        <v>25</v>
+      </c>
+      <c r="U41" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="7">
         <v>132</v>
       </c>
-      <c r="E42" s="6">
-        <v>1</v>
-      </c>
-      <c r="F42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="H42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="K42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="L42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="6">
-        <v>0</v>
-      </c>
-      <c r="N42" s="6">
-        <v>0</v>
-      </c>
-      <c r="O42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T42" s="6" t="s">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>-1</v>
+      </c>
+      <c r="G42">
+        <v>-1</v>
+      </c>
+      <c r="H42">
+        <v>-1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42">
+        <v>-1</v>
+      </c>
+      <c r="K42">
+        <v>-1</v>
+      </c>
+      <c r="L42" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>-1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q42">
+        <v>-1</v>
+      </c>
+      <c r="R42">
+        <v>-1</v>
+      </c>
+      <c r="S42" t="s">
+        <v>25</v>
+      </c>
+      <c r="T42" t="s">
         <v>118</v>
       </c>
-      <c r="U42" s="6" t="s">
+      <c r="U42" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="7">
         <v>39</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T43" s="6" t="s">
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" t="s">
+        <v>25</v>
+      </c>
+      <c r="O43" t="s">
+        <v>25</v>
+      </c>
+      <c r="P43" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>25</v>
+      </c>
+      <c r="R43" t="s">
+        <v>25</v>
+      </c>
+      <c r="S43" t="s">
+        <v>25</v>
+      </c>
+      <c r="T43" t="s">
         <v>120</v>
       </c>
-      <c r="U43" s="6" t="s">
+      <c r="U43" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>